<commit_message>
Adding Excel reader through data provider which reads all the data from excel.... this doesn't read specific cell value...
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/dsalgo.xlsx
+++ b/src/test/resources/testData/dsalgo.xlsx
@@ -1,77 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7005" activeTab="3"/>
-  </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Code" sheetId="4" r:id="rId4"/>
+    <sheet state="visible" name="LoginData" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Code" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Sheet3" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames/>
+  <calcPr/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="XFkpvDzHaf0XvYiLmI5dCjdEqUsw+SHbp4gividmxsI="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
-  <si>
-    <t>input</t>
-  </si>
-  <si>
-    <t>expectedOutput</t>
-  </si>
-  <si>
-    <t>print('Hello Selenium')</t>
-  </si>
-  <si>
-    <t>Hello Selenium</t>
-  </si>
-  <si>
-    <t>prin('Hello Selenium')</t>
-  </si>
-  <si>
-    <t>NameError: name 'prin' is not defined on line 1</t>
-  </si>
-  <si>
-    <t>UserName</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
+  <si>
+    <t>Username</t>
   </si>
   <si>
     <t>Password</t>
   </si>
   <si>
-    <t>Nirvana</t>
-  </si>
-  <si>
-    <t>archanachaya</t>
-  </si>
-  <si>
-    <t>asde@1235</t>
-  </si>
-  <si>
-    <t>tessssssttttt</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>Pyhton Code:</t>
+    <t>ninjatesterss</t>
+  </si>
+  <si>
+    <t>ninja@123</t>
+  </si>
+  <si>
+    <t>TestCase</t>
+  </si>
+  <si>
+    <t>Code</t>
   </si>
   <si>
     <t>Valid Python Code</t>
@@ -84,54 +48,6 @@
   </si>
   <si>
     <t>p("Invalid Code")</t>
-  </si>
-  <si>
-    <t>Username:</t>
-  </si>
-  <si>
-    <t>Password:</t>
-  </si>
-  <si>
-    <t>Password confirmation:</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Confirm Password</t>
-  </si>
-  <si>
-    <t>ninja tester</t>
-  </si>
-  <si>
-    <t>ninja@123</t>
-  </si>
-  <si>
-    <t>ninjatesterss</t>
-  </si>
-  <si>
-    <t>nin@1</t>
-  </si>
-  <si>
-    <t>ninja@12345</t>
-  </si>
-  <si>
-    <t>ninjatestersssss</t>
-  </si>
-  <si>
-    <t>numpyninjatester1</t>
-  </si>
-  <si>
-    <t>numpyninjatester2</t>
-  </si>
-  <si>
-    <t>numpyninjatester3</t>
-  </si>
-  <si>
-    <t>TestCase</t>
-  </si>
-  <si>
-    <t>Code</t>
   </si>
   <si>
     <t>Search the array</t>
@@ -189,936 +105,125 @@
 return sorted_squares_list;
 sortedSquares([-7,-3,2,3,11])</t>
   </si>
+  <si>
+    <t>Username:</t>
+  </si>
+  <si>
+    <t>Password:</t>
+  </si>
+  <si>
+    <t>Password confirmation:</t>
+  </si>
+  <si>
+    <t>Confirm Password</t>
+  </si>
+  <si>
+    <t>ninja tester</t>
+  </si>
+  <si>
+    <t>nin@1</t>
+  </si>
+  <si>
+    <t>ninja@12345</t>
+  </si>
+  <si>
+    <t>ninjatestersssss</t>
+  </si>
+  <si>
+    <t>numpyninjatester1</t>
+  </si>
+  <si>
+    <t>numpyninjatester2</t>
+  </si>
+  <si>
+    <t>numpyninjatester3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="24">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="5">
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.25"/>
-      <color rgb="FF000000"/>
-      <name val="docs-Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF1F1F1F"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="11.0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <sz val="8.0"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="9">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
+  <borders count="1">
+    <border/>
   </borders>
-  <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
+  <cellStyleXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  </cellStyleXfs>
+  <cellXfs count="6">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-  </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <border>
-        <top style="double">
-          <color theme="4"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-        <horizontal style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <border>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-  </dxfs>
-  <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
-    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
-      <tableStyleElement type="wholeTable" dxfId="6"/>
-      <tableStyleElement type="headerRow" dxfId="5"/>
-      <tableStyleElement type="totalRow" dxfId="4"/>
-      <tableStyleElement type="firstColumn" dxfId="3"/>
-      <tableStyleElement type="lastColumn" dxfId="2"/>
-      <tableStyleElement type="firstRowStripe" dxfId="1"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
-    </tableStyle>
-    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
-      <tableStyleElement type="headerRow" dxfId="16"/>
-      <tableStyleElement type="totalRow" dxfId="15"/>
-      <tableStyleElement type="firstRowStripe" dxfId="14"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="8"/>
-      <tableStyleElement type="pageFieldValues" dxfId="7"/>
-    </tableStyle>
-  </tableStyles>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <dxfs count="0"/>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1308,46 +413,110 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:B1000"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1" outlineLevelCol="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="26" width="9" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="36.71"/>
+    <col customWidth="1" min="2" max="2" width="35.86"/>
+    <col customWidth="1" min="3" max="6" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
+    <row r="1">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2" s="7" customFormat="1" spans="1:2">
-      <c r="A2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>3</v>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" s="7" customFormat="1" spans="1:2">
-      <c r="A3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>5</v>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" ht="141.75" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" ht="102.0" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" ht="150.75" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" ht="129.0" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -2331,79 +1500,153 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="1" orientation="landscape"/>
-  <headerFooter/>
+  <printOptions/>
+  <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
+  <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:B1000"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1" outlineLevelCol="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="27.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="19.1428571428571" customWidth="1"/>
-    <col min="3" max="26" width="9.14285714285714" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="35.86"/>
+    <col customWidth="1" min="2" max="2" width="14.43"/>
+    <col customWidth="1" min="3" max="3" width="18.14"/>
+    <col customWidth="1" min="4" max="6" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>7</v>
+    <row r="1">
+      <c r="A1" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>9</v>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>10</v>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>13</v>
+    <row r="5">
+      <c r="A5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1.23456789E9</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.23456789E9</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -3387,241 +2630,9 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="Nirvana"/>
-    <hyperlink ref="B2" r:id="rId2" display="archanachaya"/>
-    <hyperlink ref="A3" r:id="rId1" display="Nirvana"/>
-    <hyperlink ref="B3" r:id="rId2" display="asde@1235"/>
-  </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
-  <pageSetup paperSize="1" orientation="landscape"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:C13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1" outlineLevelCol="2"/>
-  <cols>
-    <col min="1" max="1" width="35.8571428571429" customWidth="1"/>
-    <col min="3" max="3" width="18.1428571428571" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" customHeight="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" customHeight="1" spans="1:1">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" customHeight="1" spans="1:1">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" customHeight="1" spans="1:3">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" customHeight="1" spans="1:3">
-      <c r="A5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" customHeight="1" spans="1:3">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" customHeight="1" spans="1:3">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7">
-        <v>1234567890</v>
-      </c>
-      <c r="C7">
-        <v>1234567890</v>
-      </c>
-    </row>
-    <row r="8" customHeight="1" spans="1:3">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" customHeight="1" spans="1:3">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" customHeight="1" spans="1:3">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" customHeight="1" spans="1:3">
-      <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" customHeight="1" spans="1:3">
-      <c r="A12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" customHeight="1" spans="1:3">
-      <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1" outlineLevelRow="6" outlineLevelCol="1"/>
-  <cols>
-    <col min="1" max="1" width="36.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="35.8571428571429" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" customHeight="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" customHeight="1" spans="1:2">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" customHeight="1" spans="1:2">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" ht="142" customHeight="1" spans="1:2">
-      <c r="A4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" ht="102" customHeight="1" spans="1:2">
-      <c r="A5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" ht="151" customHeight="1" spans="1:2">
-      <c r="A6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" ht="129" customHeight="1" spans="1:2">
-      <c r="A7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
+  <printOptions/>
+  <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
+  <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added CommonDataProvider Added Graph module update ExcelResder and Excel file
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/dsalgo.xlsx
+++ b/src/test/resources/testData/dsalgo.xlsx
@@ -4,13 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7005" activeTab="3"/>
+    <workbookView windowWidth="20490" windowHeight="7005" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Code" sheetId="4" r:id="rId4"/>
+    <sheet name="LoginData" sheetId="5" r:id="rId1"/>
+    <sheet name="login" sheetId="2" r:id="rId2"/>
+    <sheet name="Code" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,108 +29,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
   <si>
-    <t>input</t>
+    <t>Username</t>
   </si>
   <si>
-    <t>expectedOutput</t>
+    <t>Password</t>
   </si>
   <si>
-    <t>print('Hello Selenium')</t>
+    <t>ninjatesterss</t>
   </si>
   <si>
-    <t>Hello Selenium</t>
+    <t>ninja@123</t>
   </si>
   <si>
-    <t>prin('Hello Selenium')</t>
+    <t>ninjaaaa</t>
   </si>
   <si>
-    <t>NameError: name 'prin' is not defined on line 1</t>
+    <t>nin23</t>
+  </si>
+  <si>
+    <t>TestCase</t>
+  </si>
+  <si>
+    <t>DataCode</t>
   </si>
   <si>
     <t>UserName</t>
   </si>
   <si>
-    <t>Password</t>
+    <t>ValidUsernamePassword</t>
   </si>
   <si>
-    <t>Nirvana</t>
-  </si>
-  <si>
-    <t>archanachaya</t>
-  </si>
-  <si>
-    <t>asde@1235</t>
-  </si>
-  <si>
-    <t>tessssssttttt</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>Pyhton Code:</t>
-  </si>
-  <si>
-    <t>Valid Python Code</t>
+    <t>ValidPythonCode</t>
   </si>
   <si>
     <t>print("This is a valid python code")</t>
   </si>
   <si>
-    <t>Incali Python Code</t>
+    <t>InvalidPythonCode</t>
   </si>
   <si>
     <t>p("Invalid Code")</t>
-  </si>
-  <si>
-    <t>Username:</t>
-  </si>
-  <si>
-    <t>Password:</t>
-  </si>
-  <si>
-    <t>Password confirmation:</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Confirm Password</t>
-  </si>
-  <si>
-    <t>ninja tester</t>
-  </si>
-  <si>
-    <t>ninja@123</t>
-  </si>
-  <si>
-    <t>ninjatesterss</t>
-  </si>
-  <si>
-    <t>nin@1</t>
-  </si>
-  <si>
-    <t>ninja@12345</t>
-  </si>
-  <si>
-    <t>ninjatestersssss</t>
-  </si>
-  <si>
-    <t>numpyninjatester1</t>
-  </si>
-  <si>
-    <t>numpyninjatester2</t>
-  </si>
-  <si>
-    <t>numpyninjatester3</t>
-  </si>
-  <si>
-    <t>TestCase</t>
-  </si>
-  <si>
-    <t>Code</t>
   </si>
   <si>
     <t>Search the array</t>
@@ -200,12 +139,20 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -215,37 +162,9 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF1F1F1F"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -697,151 +616,146 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1315,1024 +1229,56 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B1000"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1" outlineLevelCol="1"/>
-  <cols>
-    <col min="1" max="26" width="9" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1" outlineLevelRow="4" outlineLevelCol="1"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="4" t="s">
+    <row r="1" customHeight="1" spans="1:2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" s="7" customFormat="1" spans="1:2">
-      <c r="A2" s="7" t="s">
+    <row r="2" customHeight="1" spans="1:2">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" s="7" customFormat="1" spans="1:2">
-      <c r="A3" s="7" t="s">
+    <row r="3" customHeight="1" spans="1:2">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
-    <row r="33" ht="15.75" customHeight="1"/>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
-    <row r="37" ht="15.75" customHeight="1"/>
-    <row r="38" ht="15.75" customHeight="1"/>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
-    <row r="65" ht="15.75" customHeight="1"/>
-    <row r="66" ht="15.75" customHeight="1"/>
-    <row r="67" ht="15.75" customHeight="1"/>
-    <row r="68" ht="15.75" customHeight="1"/>
-    <row r="69" ht="15.75" customHeight="1"/>
-    <row r="70" ht="15.75" customHeight="1"/>
-    <row r="71" ht="15.75" customHeight="1"/>
-    <row r="72" ht="15.75" customHeight="1"/>
-    <row r="73" ht="15.75" customHeight="1"/>
-    <row r="74" ht="15.75" customHeight="1"/>
-    <row r="75" ht="15.75" customHeight="1"/>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
-    <row r="78" ht="15.75" customHeight="1"/>
-    <row r="79" ht="15.75" customHeight="1"/>
-    <row r="80" ht="15.75" customHeight="1"/>
-    <row r="81" ht="15.75" customHeight="1"/>
-    <row r="82" ht="15.75" customHeight="1"/>
-    <row r="83" ht="15.75" customHeight="1"/>
-    <row r="84" ht="15.75" customHeight="1"/>
-    <row r="85" ht="15.75" customHeight="1"/>
-    <row r="86" ht="15.75" customHeight="1"/>
-    <row r="87" ht="15.75" customHeight="1"/>
-    <row r="88" ht="15.75" customHeight="1"/>
-    <row r="89" ht="15.75" customHeight="1"/>
-    <row r="90" ht="15.75" customHeight="1"/>
-    <row r="91" ht="15.75" customHeight="1"/>
-    <row r="92" ht="15.75" customHeight="1"/>
-    <row r="93" ht="15.75" customHeight="1"/>
-    <row r="94" ht="15.75" customHeight="1"/>
-    <row r="95" ht="15.75" customHeight="1"/>
-    <row r="96" ht="15.75" customHeight="1"/>
-    <row r="97" ht="15.75" customHeight="1"/>
-    <row r="98" ht="15.75" customHeight="1"/>
-    <row r="99" ht="15.75" customHeight="1"/>
-    <row r="100" ht="15.75" customHeight="1"/>
-    <row r="101" ht="15.75" customHeight="1"/>
-    <row r="102" ht="15.75" customHeight="1"/>
-    <row r="103" ht="15.75" customHeight="1"/>
-    <row r="104" ht="15.75" customHeight="1"/>
-    <row r="105" ht="15.75" customHeight="1"/>
-    <row r="106" ht="15.75" customHeight="1"/>
-    <row r="107" ht="15.75" customHeight="1"/>
-    <row r="108" ht="15.75" customHeight="1"/>
-    <row r="109" ht="15.75" customHeight="1"/>
-    <row r="110" ht="15.75" customHeight="1"/>
-    <row r="111" ht="15.75" customHeight="1"/>
-    <row r="112" ht="15.75" customHeight="1"/>
-    <row r="113" ht="15.75" customHeight="1"/>
-    <row r="114" ht="15.75" customHeight="1"/>
-    <row r="115" ht="15.75" customHeight="1"/>
-    <row r="116" ht="15.75" customHeight="1"/>
-    <row r="117" ht="15.75" customHeight="1"/>
-    <row r="118" ht="15.75" customHeight="1"/>
-    <row r="119" ht="15.75" customHeight="1"/>
-    <row r="120" ht="15.75" customHeight="1"/>
-    <row r="121" ht="15.75" customHeight="1"/>
-    <row r="122" ht="15.75" customHeight="1"/>
-    <row r="123" ht="15.75" customHeight="1"/>
-    <row r="124" ht="15.75" customHeight="1"/>
-    <row r="125" ht="15.75" customHeight="1"/>
-    <row r="126" ht="15.75" customHeight="1"/>
-    <row r="127" ht="15.75" customHeight="1"/>
-    <row r="128" ht="15.75" customHeight="1"/>
-    <row r="129" ht="15.75" customHeight="1"/>
-    <row r="130" ht="15.75" customHeight="1"/>
-    <row r="131" ht="15.75" customHeight="1"/>
-    <row r="132" ht="15.75" customHeight="1"/>
-    <row r="133" ht="15.75" customHeight="1"/>
-    <row r="134" ht="15.75" customHeight="1"/>
-    <row r="135" ht="15.75" customHeight="1"/>
-    <row r="136" ht="15.75" customHeight="1"/>
-    <row r="137" ht="15.75" customHeight="1"/>
-    <row r="138" ht="15.75" customHeight="1"/>
-    <row r="139" ht="15.75" customHeight="1"/>
-    <row r="140" ht="15.75" customHeight="1"/>
-    <row r="141" ht="15.75" customHeight="1"/>
-    <row r="142" ht="15.75" customHeight="1"/>
-    <row r="143" ht="15.75" customHeight="1"/>
-    <row r="144" ht="15.75" customHeight="1"/>
-    <row r="145" ht="15.75" customHeight="1"/>
-    <row r="146" ht="15.75" customHeight="1"/>
-    <row r="147" ht="15.75" customHeight="1"/>
-    <row r="148" ht="15.75" customHeight="1"/>
-    <row r="149" ht="15.75" customHeight="1"/>
-    <row r="150" ht="15.75" customHeight="1"/>
-    <row r="151" ht="15.75" customHeight="1"/>
-    <row r="152" ht="15.75" customHeight="1"/>
-    <row r="153" ht="15.75" customHeight="1"/>
-    <row r="154" ht="15.75" customHeight="1"/>
-    <row r="155" ht="15.75" customHeight="1"/>
-    <row r="156" ht="15.75" customHeight="1"/>
-    <row r="157" ht="15.75" customHeight="1"/>
-    <row r="158" ht="15.75" customHeight="1"/>
-    <row r="159" ht="15.75" customHeight="1"/>
-    <row r="160" ht="15.75" customHeight="1"/>
-    <row r="161" ht="15.75" customHeight="1"/>
-    <row r="162" ht="15.75" customHeight="1"/>
-    <row r="163" ht="15.75" customHeight="1"/>
-    <row r="164" ht="15.75" customHeight="1"/>
-    <row r="165" ht="15.75" customHeight="1"/>
-    <row r="166" ht="15.75" customHeight="1"/>
-    <row r="167" ht="15.75" customHeight="1"/>
-    <row r="168" ht="15.75" customHeight="1"/>
-    <row r="169" ht="15.75" customHeight="1"/>
-    <row r="170" ht="15.75" customHeight="1"/>
-    <row r="171" ht="15.75" customHeight="1"/>
-    <row r="172" ht="15.75" customHeight="1"/>
-    <row r="173" ht="15.75" customHeight="1"/>
-    <row r="174" ht="15.75" customHeight="1"/>
-    <row r="175" ht="15.75" customHeight="1"/>
-    <row r="176" ht="15.75" customHeight="1"/>
-    <row r="177" ht="15.75" customHeight="1"/>
-    <row r="178" ht="15.75" customHeight="1"/>
-    <row r="179" ht="15.75" customHeight="1"/>
-    <row r="180" ht="15.75" customHeight="1"/>
-    <row r="181" ht="15.75" customHeight="1"/>
-    <row r="182" ht="15.75" customHeight="1"/>
-    <row r="183" ht="15.75" customHeight="1"/>
-    <row r="184" ht="15.75" customHeight="1"/>
-    <row r="185" ht="15.75" customHeight="1"/>
-    <row r="186" ht="15.75" customHeight="1"/>
-    <row r="187" ht="15.75" customHeight="1"/>
-    <row r="188" ht="15.75" customHeight="1"/>
-    <row r="189" ht="15.75" customHeight="1"/>
-    <row r="190" ht="15.75" customHeight="1"/>
-    <row r="191" ht="15.75" customHeight="1"/>
-    <row r="192" ht="15.75" customHeight="1"/>
-    <row r="193" ht="15.75" customHeight="1"/>
-    <row r="194" ht="15.75" customHeight="1"/>
-    <row r="195" ht="15.75" customHeight="1"/>
-    <row r="196" ht="15.75" customHeight="1"/>
-    <row r="197" ht="15.75" customHeight="1"/>
-    <row r="198" ht="15.75" customHeight="1"/>
-    <row r="199" ht="15.75" customHeight="1"/>
-    <row r="200" ht="15.75" customHeight="1"/>
-    <row r="201" ht="15.75" customHeight="1"/>
-    <row r="202" ht="15.75" customHeight="1"/>
-    <row r="203" ht="15.75" customHeight="1"/>
-    <row r="204" ht="15.75" customHeight="1"/>
-    <row r="205" ht="15.75" customHeight="1"/>
-    <row r="206" ht="15.75" customHeight="1"/>
-    <row r="207" ht="15.75" customHeight="1"/>
-    <row r="208" ht="15.75" customHeight="1"/>
-    <row r="209" ht="15.75" customHeight="1"/>
-    <row r="210" ht="15.75" customHeight="1"/>
-    <row r="211" ht="15.75" customHeight="1"/>
-    <row r="212" ht="15.75" customHeight="1"/>
-    <row r="213" ht="15.75" customHeight="1"/>
-    <row r="214" ht="15.75" customHeight="1"/>
-    <row r="215" ht="15.75" customHeight="1"/>
-    <row r="216" ht="15.75" customHeight="1"/>
-    <row r="217" ht="15.75" customHeight="1"/>
-    <row r="218" ht="15.75" customHeight="1"/>
-    <row r="219" ht="15.75" customHeight="1"/>
-    <row r="220" ht="15.75" customHeight="1"/>
-    <row r="221" ht="15.75" customHeight="1"/>
-    <row r="222" ht="15.75" customHeight="1"/>
-    <row r="223" ht="15.75" customHeight="1"/>
-    <row r="224" ht="15.75" customHeight="1"/>
-    <row r="225" ht="15.75" customHeight="1"/>
-    <row r="226" ht="15.75" customHeight="1"/>
-    <row r="227" ht="15.75" customHeight="1"/>
-    <row r="228" ht="15.75" customHeight="1"/>
-    <row r="229" ht="15.75" customHeight="1"/>
-    <row r="230" ht="15.75" customHeight="1"/>
-    <row r="231" ht="15.75" customHeight="1"/>
-    <row r="232" ht="15.75" customHeight="1"/>
-    <row r="233" ht="15.75" customHeight="1"/>
-    <row r="234" ht="15.75" customHeight="1"/>
-    <row r="235" ht="15.75" customHeight="1"/>
-    <row r="236" ht="15.75" customHeight="1"/>
-    <row r="237" ht="15.75" customHeight="1"/>
-    <row r="238" ht="15.75" customHeight="1"/>
-    <row r="239" ht="15.75" customHeight="1"/>
-    <row r="240" ht="15.75" customHeight="1"/>
-    <row r="241" ht="15.75" customHeight="1"/>
-    <row r="242" ht="15.75" customHeight="1"/>
-    <row r="243" ht="15.75" customHeight="1"/>
-    <row r="244" ht="15.75" customHeight="1"/>
-    <row r="245" ht="15.75" customHeight="1"/>
-    <row r="246" ht="15.75" customHeight="1"/>
-    <row r="247" ht="15.75" customHeight="1"/>
-    <row r="248" ht="15.75" customHeight="1"/>
-    <row r="249" ht="15.75" customHeight="1"/>
-    <row r="250" ht="15.75" customHeight="1"/>
-    <row r="251" ht="15.75" customHeight="1"/>
-    <row r="252" ht="15.75" customHeight="1"/>
-    <row r="253" ht="15.75" customHeight="1"/>
-    <row r="254" ht="15.75" customHeight="1"/>
-    <row r="255" ht="15.75" customHeight="1"/>
-    <row r="256" ht="15.75" customHeight="1"/>
-    <row r="257" ht="15.75" customHeight="1"/>
-    <row r="258" ht="15.75" customHeight="1"/>
-    <row r="259" ht="15.75" customHeight="1"/>
-    <row r="260" ht="15.75" customHeight="1"/>
-    <row r="261" ht="15.75" customHeight="1"/>
-    <row r="262" ht="15.75" customHeight="1"/>
-    <row r="263" ht="15.75" customHeight="1"/>
-    <row r="264" ht="15.75" customHeight="1"/>
-    <row r="265" ht="15.75" customHeight="1"/>
-    <row r="266" ht="15.75" customHeight="1"/>
-    <row r="267" ht="15.75" customHeight="1"/>
-    <row r="268" ht="15.75" customHeight="1"/>
-    <row r="269" ht="15.75" customHeight="1"/>
-    <row r="270" ht="15.75" customHeight="1"/>
-    <row r="271" ht="15.75" customHeight="1"/>
-    <row r="272" ht="15.75" customHeight="1"/>
-    <row r="273" ht="15.75" customHeight="1"/>
-    <row r="274" ht="15.75" customHeight="1"/>
-    <row r="275" ht="15.75" customHeight="1"/>
-    <row r="276" ht="15.75" customHeight="1"/>
-    <row r="277" ht="15.75" customHeight="1"/>
-    <row r="278" ht="15.75" customHeight="1"/>
-    <row r="279" ht="15.75" customHeight="1"/>
-    <row r="280" ht="15.75" customHeight="1"/>
-    <row r="281" ht="15.75" customHeight="1"/>
-    <row r="282" ht="15.75" customHeight="1"/>
-    <row r="283" ht="15.75" customHeight="1"/>
-    <row r="284" ht="15.75" customHeight="1"/>
-    <row r="285" ht="15.75" customHeight="1"/>
-    <row r="286" ht="15.75" customHeight="1"/>
-    <row r="287" ht="15.75" customHeight="1"/>
-    <row r="288" ht="15.75" customHeight="1"/>
-    <row r="289" ht="15.75" customHeight="1"/>
-    <row r="290" ht="15.75" customHeight="1"/>
-    <row r="291" ht="15.75" customHeight="1"/>
-    <row r="292" ht="15.75" customHeight="1"/>
-    <row r="293" ht="15.75" customHeight="1"/>
-    <row r="294" ht="15.75" customHeight="1"/>
-    <row r="295" ht="15.75" customHeight="1"/>
-    <row r="296" ht="15.75" customHeight="1"/>
-    <row r="297" ht="15.75" customHeight="1"/>
-    <row r="298" ht="15.75" customHeight="1"/>
-    <row r="299" ht="15.75" customHeight="1"/>
-    <row r="300" ht="15.75" customHeight="1"/>
-    <row r="301" ht="15.75" customHeight="1"/>
-    <row r="302" ht="15.75" customHeight="1"/>
-    <row r="303" ht="15.75" customHeight="1"/>
-    <row r="304" ht="15.75" customHeight="1"/>
-    <row r="305" ht="15.75" customHeight="1"/>
-    <row r="306" ht="15.75" customHeight="1"/>
-    <row r="307" ht="15.75" customHeight="1"/>
-    <row r="308" ht="15.75" customHeight="1"/>
-    <row r="309" ht="15.75" customHeight="1"/>
-    <row r="310" ht="15.75" customHeight="1"/>
-    <row r="311" ht="15.75" customHeight="1"/>
-    <row r="312" ht="15.75" customHeight="1"/>
-    <row r="313" ht="15.75" customHeight="1"/>
-    <row r="314" ht="15.75" customHeight="1"/>
-    <row r="315" ht="15.75" customHeight="1"/>
-    <row r="316" ht="15.75" customHeight="1"/>
-    <row r="317" ht="15.75" customHeight="1"/>
-    <row r="318" ht="15.75" customHeight="1"/>
-    <row r="319" ht="15.75" customHeight="1"/>
-    <row r="320" ht="15.75" customHeight="1"/>
-    <row r="321" ht="15.75" customHeight="1"/>
-    <row r="322" ht="15.75" customHeight="1"/>
-    <row r="323" ht="15.75" customHeight="1"/>
-    <row r="324" ht="15.75" customHeight="1"/>
-    <row r="325" ht="15.75" customHeight="1"/>
-    <row r="326" ht="15.75" customHeight="1"/>
-    <row r="327" ht="15.75" customHeight="1"/>
-    <row r="328" ht="15.75" customHeight="1"/>
-    <row r="329" ht="15.75" customHeight="1"/>
-    <row r="330" ht="15.75" customHeight="1"/>
-    <row r="331" ht="15.75" customHeight="1"/>
-    <row r="332" ht="15.75" customHeight="1"/>
-    <row r="333" ht="15.75" customHeight="1"/>
-    <row r="334" ht="15.75" customHeight="1"/>
-    <row r="335" ht="15.75" customHeight="1"/>
-    <row r="336" ht="15.75" customHeight="1"/>
-    <row r="337" ht="15.75" customHeight="1"/>
-    <row r="338" ht="15.75" customHeight="1"/>
-    <row r="339" ht="15.75" customHeight="1"/>
-    <row r="340" ht="15.75" customHeight="1"/>
-    <row r="341" ht="15.75" customHeight="1"/>
-    <row r="342" ht="15.75" customHeight="1"/>
-    <row r="343" ht="15.75" customHeight="1"/>
-    <row r="344" ht="15.75" customHeight="1"/>
-    <row r="345" ht="15.75" customHeight="1"/>
-    <row r="346" ht="15.75" customHeight="1"/>
-    <row r="347" ht="15.75" customHeight="1"/>
-    <row r="348" ht="15.75" customHeight="1"/>
-    <row r="349" ht="15.75" customHeight="1"/>
-    <row r="350" ht="15.75" customHeight="1"/>
-    <row r="351" ht="15.75" customHeight="1"/>
-    <row r="352" ht="15.75" customHeight="1"/>
-    <row r="353" ht="15.75" customHeight="1"/>
-    <row r="354" ht="15.75" customHeight="1"/>
-    <row r="355" ht="15.75" customHeight="1"/>
-    <row r="356" ht="15.75" customHeight="1"/>
-    <row r="357" ht="15.75" customHeight="1"/>
-    <row r="358" ht="15.75" customHeight="1"/>
-    <row r="359" ht="15.75" customHeight="1"/>
-    <row r="360" ht="15.75" customHeight="1"/>
-    <row r="361" ht="15.75" customHeight="1"/>
-    <row r="362" ht="15.75" customHeight="1"/>
-    <row r="363" ht="15.75" customHeight="1"/>
-    <row r="364" ht="15.75" customHeight="1"/>
-    <row r="365" ht="15.75" customHeight="1"/>
-    <row r="366" ht="15.75" customHeight="1"/>
-    <row r="367" ht="15.75" customHeight="1"/>
-    <row r="368" ht="15.75" customHeight="1"/>
-    <row r="369" ht="15.75" customHeight="1"/>
-    <row r="370" ht="15.75" customHeight="1"/>
-    <row r="371" ht="15.75" customHeight="1"/>
-    <row r="372" ht="15.75" customHeight="1"/>
-    <row r="373" ht="15.75" customHeight="1"/>
-    <row r="374" ht="15.75" customHeight="1"/>
-    <row r="375" ht="15.75" customHeight="1"/>
-    <row r="376" ht="15.75" customHeight="1"/>
-    <row r="377" ht="15.75" customHeight="1"/>
-    <row r="378" ht="15.75" customHeight="1"/>
-    <row r="379" ht="15.75" customHeight="1"/>
-    <row r="380" ht="15.75" customHeight="1"/>
-    <row r="381" ht="15.75" customHeight="1"/>
-    <row r="382" ht="15.75" customHeight="1"/>
-    <row r="383" ht="15.75" customHeight="1"/>
-    <row r="384" ht="15.75" customHeight="1"/>
-    <row r="385" ht="15.75" customHeight="1"/>
-    <row r="386" ht="15.75" customHeight="1"/>
-    <row r="387" ht="15.75" customHeight="1"/>
-    <row r="388" ht="15.75" customHeight="1"/>
-    <row r="389" ht="15.75" customHeight="1"/>
-    <row r="390" ht="15.75" customHeight="1"/>
-    <row r="391" ht="15.75" customHeight="1"/>
-    <row r="392" ht="15.75" customHeight="1"/>
-    <row r="393" ht="15.75" customHeight="1"/>
-    <row r="394" ht="15.75" customHeight="1"/>
-    <row r="395" ht="15.75" customHeight="1"/>
-    <row r="396" ht="15.75" customHeight="1"/>
-    <row r="397" ht="15.75" customHeight="1"/>
-    <row r="398" ht="15.75" customHeight="1"/>
-    <row r="399" ht="15.75" customHeight="1"/>
-    <row r="400" ht="15.75" customHeight="1"/>
-    <row r="401" ht="15.75" customHeight="1"/>
-    <row r="402" ht="15.75" customHeight="1"/>
-    <row r="403" ht="15.75" customHeight="1"/>
-    <row r="404" ht="15.75" customHeight="1"/>
-    <row r="405" ht="15.75" customHeight="1"/>
-    <row r="406" ht="15.75" customHeight="1"/>
-    <row r="407" ht="15.75" customHeight="1"/>
-    <row r="408" ht="15.75" customHeight="1"/>
-    <row r="409" ht="15.75" customHeight="1"/>
-    <row r="410" ht="15.75" customHeight="1"/>
-    <row r="411" ht="15.75" customHeight="1"/>
-    <row r="412" ht="15.75" customHeight="1"/>
-    <row r="413" ht="15.75" customHeight="1"/>
-    <row r="414" ht="15.75" customHeight="1"/>
-    <row r="415" ht="15.75" customHeight="1"/>
-    <row r="416" ht="15.75" customHeight="1"/>
-    <row r="417" ht="15.75" customHeight="1"/>
-    <row r="418" ht="15.75" customHeight="1"/>
-    <row r="419" ht="15.75" customHeight="1"/>
-    <row r="420" ht="15.75" customHeight="1"/>
-    <row r="421" ht="15.75" customHeight="1"/>
-    <row r="422" ht="15.75" customHeight="1"/>
-    <row r="423" ht="15.75" customHeight="1"/>
-    <row r="424" ht="15.75" customHeight="1"/>
-    <row r="425" ht="15.75" customHeight="1"/>
-    <row r="426" ht="15.75" customHeight="1"/>
-    <row r="427" ht="15.75" customHeight="1"/>
-    <row r="428" ht="15.75" customHeight="1"/>
-    <row r="429" ht="15.75" customHeight="1"/>
-    <row r="430" ht="15.75" customHeight="1"/>
-    <row r="431" ht="15.75" customHeight="1"/>
-    <row r="432" ht="15.75" customHeight="1"/>
-    <row r="433" ht="15.75" customHeight="1"/>
-    <row r="434" ht="15.75" customHeight="1"/>
-    <row r="435" ht="15.75" customHeight="1"/>
-    <row r="436" ht="15.75" customHeight="1"/>
-    <row r="437" ht="15.75" customHeight="1"/>
-    <row r="438" ht="15.75" customHeight="1"/>
-    <row r="439" ht="15.75" customHeight="1"/>
-    <row r="440" ht="15.75" customHeight="1"/>
-    <row r="441" ht="15.75" customHeight="1"/>
-    <row r="442" ht="15.75" customHeight="1"/>
-    <row r="443" ht="15.75" customHeight="1"/>
-    <row r="444" ht="15.75" customHeight="1"/>
-    <row r="445" ht="15.75" customHeight="1"/>
-    <row r="446" ht="15.75" customHeight="1"/>
-    <row r="447" ht="15.75" customHeight="1"/>
-    <row r="448" ht="15.75" customHeight="1"/>
-    <row r="449" ht="15.75" customHeight="1"/>
-    <row r="450" ht="15.75" customHeight="1"/>
-    <row r="451" ht="15.75" customHeight="1"/>
-    <row r="452" ht="15.75" customHeight="1"/>
-    <row r="453" ht="15.75" customHeight="1"/>
-    <row r="454" ht="15.75" customHeight="1"/>
-    <row r="455" ht="15.75" customHeight="1"/>
-    <row r="456" ht="15.75" customHeight="1"/>
-    <row r="457" ht="15.75" customHeight="1"/>
-    <row r="458" ht="15.75" customHeight="1"/>
-    <row r="459" ht="15.75" customHeight="1"/>
-    <row r="460" ht="15.75" customHeight="1"/>
-    <row r="461" ht="15.75" customHeight="1"/>
-    <row r="462" ht="15.75" customHeight="1"/>
-    <row r="463" ht="15.75" customHeight="1"/>
-    <row r="464" ht="15.75" customHeight="1"/>
-    <row r="465" ht="15.75" customHeight="1"/>
-    <row r="466" ht="15.75" customHeight="1"/>
-    <row r="467" ht="15.75" customHeight="1"/>
-    <row r="468" ht="15.75" customHeight="1"/>
-    <row r="469" ht="15.75" customHeight="1"/>
-    <row r="470" ht="15.75" customHeight="1"/>
-    <row r="471" ht="15.75" customHeight="1"/>
-    <row r="472" ht="15.75" customHeight="1"/>
-    <row r="473" ht="15.75" customHeight="1"/>
-    <row r="474" ht="15.75" customHeight="1"/>
-    <row r="475" ht="15.75" customHeight="1"/>
-    <row r="476" ht="15.75" customHeight="1"/>
-    <row r="477" ht="15.75" customHeight="1"/>
-    <row r="478" ht="15.75" customHeight="1"/>
-    <row r="479" ht="15.75" customHeight="1"/>
-    <row r="480" ht="15.75" customHeight="1"/>
-    <row r="481" ht="15.75" customHeight="1"/>
-    <row r="482" ht="15.75" customHeight="1"/>
-    <row r="483" ht="15.75" customHeight="1"/>
-    <row r="484" ht="15.75" customHeight="1"/>
-    <row r="485" ht="15.75" customHeight="1"/>
-    <row r="486" ht="15.75" customHeight="1"/>
-    <row r="487" ht="15.75" customHeight="1"/>
-    <row r="488" ht="15.75" customHeight="1"/>
-    <row r="489" ht="15.75" customHeight="1"/>
-    <row r="490" ht="15.75" customHeight="1"/>
-    <row r="491" ht="15.75" customHeight="1"/>
-    <row r="492" ht="15.75" customHeight="1"/>
-    <row r="493" ht="15.75" customHeight="1"/>
-    <row r="494" ht="15.75" customHeight="1"/>
-    <row r="495" ht="15.75" customHeight="1"/>
-    <row r="496" ht="15.75" customHeight="1"/>
-    <row r="497" ht="15.75" customHeight="1"/>
-    <row r="498" ht="15.75" customHeight="1"/>
-    <row r="499" ht="15.75" customHeight="1"/>
-    <row r="500" ht="15.75" customHeight="1"/>
-    <row r="501" ht="15.75" customHeight="1"/>
-    <row r="502" ht="15.75" customHeight="1"/>
-    <row r="503" ht="15.75" customHeight="1"/>
-    <row r="504" ht="15.75" customHeight="1"/>
-    <row r="505" ht="15.75" customHeight="1"/>
-    <row r="506" ht="15.75" customHeight="1"/>
-    <row r="507" ht="15.75" customHeight="1"/>
-    <row r="508" ht="15.75" customHeight="1"/>
-    <row r="509" ht="15.75" customHeight="1"/>
-    <row r="510" ht="15.75" customHeight="1"/>
-    <row r="511" ht="15.75" customHeight="1"/>
-    <row r="512" ht="15.75" customHeight="1"/>
-    <row r="513" ht="15.75" customHeight="1"/>
-    <row r="514" ht="15.75" customHeight="1"/>
-    <row r="515" ht="15.75" customHeight="1"/>
-    <row r="516" ht="15.75" customHeight="1"/>
-    <row r="517" ht="15.75" customHeight="1"/>
-    <row r="518" ht="15.75" customHeight="1"/>
-    <row r="519" ht="15.75" customHeight="1"/>
-    <row r="520" ht="15.75" customHeight="1"/>
-    <row r="521" ht="15.75" customHeight="1"/>
-    <row r="522" ht="15.75" customHeight="1"/>
-    <row r="523" ht="15.75" customHeight="1"/>
-    <row r="524" ht="15.75" customHeight="1"/>
-    <row r="525" ht="15.75" customHeight="1"/>
-    <row r="526" ht="15.75" customHeight="1"/>
-    <row r="527" ht="15.75" customHeight="1"/>
-    <row r="528" ht="15.75" customHeight="1"/>
-    <row r="529" ht="15.75" customHeight="1"/>
-    <row r="530" ht="15.75" customHeight="1"/>
-    <row r="531" ht="15.75" customHeight="1"/>
-    <row r="532" ht="15.75" customHeight="1"/>
-    <row r="533" ht="15.75" customHeight="1"/>
-    <row r="534" ht="15.75" customHeight="1"/>
-    <row r="535" ht="15.75" customHeight="1"/>
-    <row r="536" ht="15.75" customHeight="1"/>
-    <row r="537" ht="15.75" customHeight="1"/>
-    <row r="538" ht="15.75" customHeight="1"/>
-    <row r="539" ht="15.75" customHeight="1"/>
-    <row r="540" ht="15.75" customHeight="1"/>
-    <row r="541" ht="15.75" customHeight="1"/>
-    <row r="542" ht="15.75" customHeight="1"/>
-    <row r="543" ht="15.75" customHeight="1"/>
-    <row r="544" ht="15.75" customHeight="1"/>
-    <row r="545" ht="15.75" customHeight="1"/>
-    <row r="546" ht="15.75" customHeight="1"/>
-    <row r="547" ht="15.75" customHeight="1"/>
-    <row r="548" ht="15.75" customHeight="1"/>
-    <row r="549" ht="15.75" customHeight="1"/>
-    <row r="550" ht="15.75" customHeight="1"/>
-    <row r="551" ht="15.75" customHeight="1"/>
-    <row r="552" ht="15.75" customHeight="1"/>
-    <row r="553" ht="15.75" customHeight="1"/>
-    <row r="554" ht="15.75" customHeight="1"/>
-    <row r="555" ht="15.75" customHeight="1"/>
-    <row r="556" ht="15.75" customHeight="1"/>
-    <row r="557" ht="15.75" customHeight="1"/>
-    <row r="558" ht="15.75" customHeight="1"/>
-    <row r="559" ht="15.75" customHeight="1"/>
-    <row r="560" ht="15.75" customHeight="1"/>
-    <row r="561" ht="15.75" customHeight="1"/>
-    <row r="562" ht="15.75" customHeight="1"/>
-    <row r="563" ht="15.75" customHeight="1"/>
-    <row r="564" ht="15.75" customHeight="1"/>
-    <row r="565" ht="15.75" customHeight="1"/>
-    <row r="566" ht="15.75" customHeight="1"/>
-    <row r="567" ht="15.75" customHeight="1"/>
-    <row r="568" ht="15.75" customHeight="1"/>
-    <row r="569" ht="15.75" customHeight="1"/>
-    <row r="570" ht="15.75" customHeight="1"/>
-    <row r="571" ht="15.75" customHeight="1"/>
-    <row r="572" ht="15.75" customHeight="1"/>
-    <row r="573" ht="15.75" customHeight="1"/>
-    <row r="574" ht="15.75" customHeight="1"/>
-    <row r="575" ht="15.75" customHeight="1"/>
-    <row r="576" ht="15.75" customHeight="1"/>
-    <row r="577" ht="15.75" customHeight="1"/>
-    <row r="578" ht="15.75" customHeight="1"/>
-    <row r="579" ht="15.75" customHeight="1"/>
-    <row r="580" ht="15.75" customHeight="1"/>
-    <row r="581" ht="15.75" customHeight="1"/>
-    <row r="582" ht="15.75" customHeight="1"/>
-    <row r="583" ht="15.75" customHeight="1"/>
-    <row r="584" ht="15.75" customHeight="1"/>
-    <row r="585" ht="15.75" customHeight="1"/>
-    <row r="586" ht="15.75" customHeight="1"/>
-    <row r="587" ht="15.75" customHeight="1"/>
-    <row r="588" ht="15.75" customHeight="1"/>
-    <row r="589" ht="15.75" customHeight="1"/>
-    <row r="590" ht="15.75" customHeight="1"/>
-    <row r="591" ht="15.75" customHeight="1"/>
-    <row r="592" ht="15.75" customHeight="1"/>
-    <row r="593" ht="15.75" customHeight="1"/>
-    <row r="594" ht="15.75" customHeight="1"/>
-    <row r="595" ht="15.75" customHeight="1"/>
-    <row r="596" ht="15.75" customHeight="1"/>
-    <row r="597" ht="15.75" customHeight="1"/>
-    <row r="598" ht="15.75" customHeight="1"/>
-    <row r="599" ht="15.75" customHeight="1"/>
-    <row r="600" ht="15.75" customHeight="1"/>
-    <row r="601" ht="15.75" customHeight="1"/>
-    <row r="602" ht="15.75" customHeight="1"/>
-    <row r="603" ht="15.75" customHeight="1"/>
-    <row r="604" ht="15.75" customHeight="1"/>
-    <row r="605" ht="15.75" customHeight="1"/>
-    <row r="606" ht="15.75" customHeight="1"/>
-    <row r="607" ht="15.75" customHeight="1"/>
-    <row r="608" ht="15.75" customHeight="1"/>
-    <row r="609" ht="15.75" customHeight="1"/>
-    <row r="610" ht="15.75" customHeight="1"/>
-    <row r="611" ht="15.75" customHeight="1"/>
-    <row r="612" ht="15.75" customHeight="1"/>
-    <row r="613" ht="15.75" customHeight="1"/>
-    <row r="614" ht="15.75" customHeight="1"/>
-    <row r="615" ht="15.75" customHeight="1"/>
-    <row r="616" ht="15.75" customHeight="1"/>
-    <row r="617" ht="15.75" customHeight="1"/>
-    <row r="618" ht="15.75" customHeight="1"/>
-    <row r="619" ht="15.75" customHeight="1"/>
-    <row r="620" ht="15.75" customHeight="1"/>
-    <row r="621" ht="15.75" customHeight="1"/>
-    <row r="622" ht="15.75" customHeight="1"/>
-    <row r="623" ht="15.75" customHeight="1"/>
-    <row r="624" ht="15.75" customHeight="1"/>
-    <row r="625" ht="15.75" customHeight="1"/>
-    <row r="626" ht="15.75" customHeight="1"/>
-    <row r="627" ht="15.75" customHeight="1"/>
-    <row r="628" ht="15.75" customHeight="1"/>
-    <row r="629" ht="15.75" customHeight="1"/>
-    <row r="630" ht="15.75" customHeight="1"/>
-    <row r="631" ht="15.75" customHeight="1"/>
-    <row r="632" ht="15.75" customHeight="1"/>
-    <row r="633" ht="15.75" customHeight="1"/>
-    <row r="634" ht="15.75" customHeight="1"/>
-    <row r="635" ht="15.75" customHeight="1"/>
-    <row r="636" ht="15.75" customHeight="1"/>
-    <row r="637" ht="15.75" customHeight="1"/>
-    <row r="638" ht="15.75" customHeight="1"/>
-    <row r="639" ht="15.75" customHeight="1"/>
-    <row r="640" ht="15.75" customHeight="1"/>
-    <row r="641" ht="15.75" customHeight="1"/>
-    <row r="642" ht="15.75" customHeight="1"/>
-    <row r="643" ht="15.75" customHeight="1"/>
-    <row r="644" ht="15.75" customHeight="1"/>
-    <row r="645" ht="15.75" customHeight="1"/>
-    <row r="646" ht="15.75" customHeight="1"/>
-    <row r="647" ht="15.75" customHeight="1"/>
-    <row r="648" ht="15.75" customHeight="1"/>
-    <row r="649" ht="15.75" customHeight="1"/>
-    <row r="650" ht="15.75" customHeight="1"/>
-    <row r="651" ht="15.75" customHeight="1"/>
-    <row r="652" ht="15.75" customHeight="1"/>
-    <row r="653" ht="15.75" customHeight="1"/>
-    <row r="654" ht="15.75" customHeight="1"/>
-    <row r="655" ht="15.75" customHeight="1"/>
-    <row r="656" ht="15.75" customHeight="1"/>
-    <row r="657" ht="15.75" customHeight="1"/>
-    <row r="658" ht="15.75" customHeight="1"/>
-    <row r="659" ht="15.75" customHeight="1"/>
-    <row r="660" ht="15.75" customHeight="1"/>
-    <row r="661" ht="15.75" customHeight="1"/>
-    <row r="662" ht="15.75" customHeight="1"/>
-    <row r="663" ht="15.75" customHeight="1"/>
-    <row r="664" ht="15.75" customHeight="1"/>
-    <row r="665" ht="15.75" customHeight="1"/>
-    <row r="666" ht="15.75" customHeight="1"/>
-    <row r="667" ht="15.75" customHeight="1"/>
-    <row r="668" ht="15.75" customHeight="1"/>
-    <row r="669" ht="15.75" customHeight="1"/>
-    <row r="670" ht="15.75" customHeight="1"/>
-    <row r="671" ht="15.75" customHeight="1"/>
-    <row r="672" ht="15.75" customHeight="1"/>
-    <row r="673" ht="15.75" customHeight="1"/>
-    <row r="674" ht="15.75" customHeight="1"/>
-    <row r="675" ht="15.75" customHeight="1"/>
-    <row r="676" ht="15.75" customHeight="1"/>
-    <row r="677" ht="15.75" customHeight="1"/>
-    <row r="678" ht="15.75" customHeight="1"/>
-    <row r="679" ht="15.75" customHeight="1"/>
-    <row r="680" ht="15.75" customHeight="1"/>
-    <row r="681" ht="15.75" customHeight="1"/>
-    <row r="682" ht="15.75" customHeight="1"/>
-    <row r="683" ht="15.75" customHeight="1"/>
-    <row r="684" ht="15.75" customHeight="1"/>
-    <row r="685" ht="15.75" customHeight="1"/>
-    <row r="686" ht="15.75" customHeight="1"/>
-    <row r="687" ht="15.75" customHeight="1"/>
-    <row r="688" ht="15.75" customHeight="1"/>
-    <row r="689" ht="15.75" customHeight="1"/>
-    <row r="690" ht="15.75" customHeight="1"/>
-    <row r="691" ht="15.75" customHeight="1"/>
-    <row r="692" ht="15.75" customHeight="1"/>
-    <row r="693" ht="15.75" customHeight="1"/>
-    <row r="694" ht="15.75" customHeight="1"/>
-    <row r="695" ht="15.75" customHeight="1"/>
-    <row r="696" ht="15.75" customHeight="1"/>
-    <row r="697" ht="15.75" customHeight="1"/>
-    <row r="698" ht="15.75" customHeight="1"/>
-    <row r="699" ht="15.75" customHeight="1"/>
-    <row r="700" ht="15.75" customHeight="1"/>
-    <row r="701" ht="15.75" customHeight="1"/>
-    <row r="702" ht="15.75" customHeight="1"/>
-    <row r="703" ht="15.75" customHeight="1"/>
-    <row r="704" ht="15.75" customHeight="1"/>
-    <row r="705" ht="15.75" customHeight="1"/>
-    <row r="706" ht="15.75" customHeight="1"/>
-    <row r="707" ht="15.75" customHeight="1"/>
-    <row r="708" ht="15.75" customHeight="1"/>
-    <row r="709" ht="15.75" customHeight="1"/>
-    <row r="710" ht="15.75" customHeight="1"/>
-    <row r="711" ht="15.75" customHeight="1"/>
-    <row r="712" ht="15.75" customHeight="1"/>
-    <row r="713" ht="15.75" customHeight="1"/>
-    <row r="714" ht="15.75" customHeight="1"/>
-    <row r="715" ht="15.75" customHeight="1"/>
-    <row r="716" ht="15.75" customHeight="1"/>
-    <row r="717" ht="15.75" customHeight="1"/>
-    <row r="718" ht="15.75" customHeight="1"/>
-    <row r="719" ht="15.75" customHeight="1"/>
-    <row r="720" ht="15.75" customHeight="1"/>
-    <row r="721" ht="15.75" customHeight="1"/>
-    <row r="722" ht="15.75" customHeight="1"/>
-    <row r="723" ht="15.75" customHeight="1"/>
-    <row r="724" ht="15.75" customHeight="1"/>
-    <row r="725" ht="15.75" customHeight="1"/>
-    <row r="726" ht="15.75" customHeight="1"/>
-    <row r="727" ht="15.75" customHeight="1"/>
-    <row r="728" ht="15.75" customHeight="1"/>
-    <row r="729" ht="15.75" customHeight="1"/>
-    <row r="730" ht="15.75" customHeight="1"/>
-    <row r="731" ht="15.75" customHeight="1"/>
-    <row r="732" ht="15.75" customHeight="1"/>
-    <row r="733" ht="15.75" customHeight="1"/>
-    <row r="734" ht="15.75" customHeight="1"/>
-    <row r="735" ht="15.75" customHeight="1"/>
-    <row r="736" ht="15.75" customHeight="1"/>
-    <row r="737" ht="15.75" customHeight="1"/>
-    <row r="738" ht="15.75" customHeight="1"/>
-    <row r="739" ht="15.75" customHeight="1"/>
-    <row r="740" ht="15.75" customHeight="1"/>
-    <row r="741" ht="15.75" customHeight="1"/>
-    <row r="742" ht="15.75" customHeight="1"/>
-    <row r="743" ht="15.75" customHeight="1"/>
-    <row r="744" ht="15.75" customHeight="1"/>
-    <row r="745" ht="15.75" customHeight="1"/>
-    <row r="746" ht="15.75" customHeight="1"/>
-    <row r="747" ht="15.75" customHeight="1"/>
-    <row r="748" ht="15.75" customHeight="1"/>
-    <row r="749" ht="15.75" customHeight="1"/>
-    <row r="750" ht="15.75" customHeight="1"/>
-    <row r="751" ht="15.75" customHeight="1"/>
-    <row r="752" ht="15.75" customHeight="1"/>
-    <row r="753" ht="15.75" customHeight="1"/>
-    <row r="754" ht="15.75" customHeight="1"/>
-    <row r="755" ht="15.75" customHeight="1"/>
-    <row r="756" ht="15.75" customHeight="1"/>
-    <row r="757" ht="15.75" customHeight="1"/>
-    <row r="758" ht="15.75" customHeight="1"/>
-    <row r="759" ht="15.75" customHeight="1"/>
-    <row r="760" ht="15.75" customHeight="1"/>
-    <row r="761" ht="15.75" customHeight="1"/>
-    <row r="762" ht="15.75" customHeight="1"/>
-    <row r="763" ht="15.75" customHeight="1"/>
-    <row r="764" ht="15.75" customHeight="1"/>
-    <row r="765" ht="15.75" customHeight="1"/>
-    <row r="766" ht="15.75" customHeight="1"/>
-    <row r="767" ht="15.75" customHeight="1"/>
-    <row r="768" ht="15.75" customHeight="1"/>
-    <row r="769" ht="15.75" customHeight="1"/>
-    <row r="770" ht="15.75" customHeight="1"/>
-    <row r="771" ht="15.75" customHeight="1"/>
-    <row r="772" ht="15.75" customHeight="1"/>
-    <row r="773" ht="15.75" customHeight="1"/>
-    <row r="774" ht="15.75" customHeight="1"/>
-    <row r="775" ht="15.75" customHeight="1"/>
-    <row r="776" ht="15.75" customHeight="1"/>
-    <row r="777" ht="15.75" customHeight="1"/>
-    <row r="778" ht="15.75" customHeight="1"/>
-    <row r="779" ht="15.75" customHeight="1"/>
-    <row r="780" ht="15.75" customHeight="1"/>
-    <row r="781" ht="15.75" customHeight="1"/>
-    <row r="782" ht="15.75" customHeight="1"/>
-    <row r="783" ht="15.75" customHeight="1"/>
-    <row r="784" ht="15.75" customHeight="1"/>
-    <row r="785" ht="15.75" customHeight="1"/>
-    <row r="786" ht="15.75" customHeight="1"/>
-    <row r="787" ht="15.75" customHeight="1"/>
-    <row r="788" ht="15.75" customHeight="1"/>
-    <row r="789" ht="15.75" customHeight="1"/>
-    <row r="790" ht="15.75" customHeight="1"/>
-    <row r="791" ht="15.75" customHeight="1"/>
-    <row r="792" ht="15.75" customHeight="1"/>
-    <row r="793" ht="15.75" customHeight="1"/>
-    <row r="794" ht="15.75" customHeight="1"/>
-    <row r="795" ht="15.75" customHeight="1"/>
-    <row r="796" ht="15.75" customHeight="1"/>
-    <row r="797" ht="15.75" customHeight="1"/>
-    <row r="798" ht="15.75" customHeight="1"/>
-    <row r="799" ht="15.75" customHeight="1"/>
-    <row r="800" ht="15.75" customHeight="1"/>
-    <row r="801" ht="15.75" customHeight="1"/>
-    <row r="802" ht="15.75" customHeight="1"/>
-    <row r="803" ht="15.75" customHeight="1"/>
-    <row r="804" ht="15.75" customHeight="1"/>
-    <row r="805" ht="15.75" customHeight="1"/>
-    <row r="806" ht="15.75" customHeight="1"/>
-    <row r="807" ht="15.75" customHeight="1"/>
-    <row r="808" ht="15.75" customHeight="1"/>
-    <row r="809" ht="15.75" customHeight="1"/>
-    <row r="810" ht="15.75" customHeight="1"/>
-    <row r="811" ht="15.75" customHeight="1"/>
-    <row r="812" ht="15.75" customHeight="1"/>
-    <row r="813" ht="15.75" customHeight="1"/>
-    <row r="814" ht="15.75" customHeight="1"/>
-    <row r="815" ht="15.75" customHeight="1"/>
-    <row r="816" ht="15.75" customHeight="1"/>
-    <row r="817" ht="15.75" customHeight="1"/>
-    <row r="818" ht="15.75" customHeight="1"/>
-    <row r="819" ht="15.75" customHeight="1"/>
-    <row r="820" ht="15.75" customHeight="1"/>
-    <row r="821" ht="15.75" customHeight="1"/>
-    <row r="822" ht="15.75" customHeight="1"/>
-    <row r="823" ht="15.75" customHeight="1"/>
-    <row r="824" ht="15.75" customHeight="1"/>
-    <row r="825" ht="15.75" customHeight="1"/>
-    <row r="826" ht="15.75" customHeight="1"/>
-    <row r="827" ht="15.75" customHeight="1"/>
-    <row r="828" ht="15.75" customHeight="1"/>
-    <row r="829" ht="15.75" customHeight="1"/>
-    <row r="830" ht="15.75" customHeight="1"/>
-    <row r="831" ht="15.75" customHeight="1"/>
-    <row r="832" ht="15.75" customHeight="1"/>
-    <row r="833" ht="15.75" customHeight="1"/>
-    <row r="834" ht="15.75" customHeight="1"/>
-    <row r="835" ht="15.75" customHeight="1"/>
-    <row r="836" ht="15.75" customHeight="1"/>
-    <row r="837" ht="15.75" customHeight="1"/>
-    <row r="838" ht="15.75" customHeight="1"/>
-    <row r="839" ht="15.75" customHeight="1"/>
-    <row r="840" ht="15.75" customHeight="1"/>
-    <row r="841" ht="15.75" customHeight="1"/>
-    <row r="842" ht="15.75" customHeight="1"/>
-    <row r="843" ht="15.75" customHeight="1"/>
-    <row r="844" ht="15.75" customHeight="1"/>
-    <row r="845" ht="15.75" customHeight="1"/>
-    <row r="846" ht="15.75" customHeight="1"/>
-    <row r="847" ht="15.75" customHeight="1"/>
-    <row r="848" ht="15.75" customHeight="1"/>
-    <row r="849" ht="15.75" customHeight="1"/>
-    <row r="850" ht="15.75" customHeight="1"/>
-    <row r="851" ht="15.75" customHeight="1"/>
-    <row r="852" ht="15.75" customHeight="1"/>
-    <row r="853" ht="15.75" customHeight="1"/>
-    <row r="854" ht="15.75" customHeight="1"/>
-    <row r="855" ht="15.75" customHeight="1"/>
-    <row r="856" ht="15.75" customHeight="1"/>
-    <row r="857" ht="15.75" customHeight="1"/>
-    <row r="858" ht="15.75" customHeight="1"/>
-    <row r="859" ht="15.75" customHeight="1"/>
-    <row r="860" ht="15.75" customHeight="1"/>
-    <row r="861" ht="15.75" customHeight="1"/>
-    <row r="862" ht="15.75" customHeight="1"/>
-    <row r="863" ht="15.75" customHeight="1"/>
-    <row r="864" ht="15.75" customHeight="1"/>
-    <row r="865" ht="15.75" customHeight="1"/>
-    <row r="866" ht="15.75" customHeight="1"/>
-    <row r="867" ht="15.75" customHeight="1"/>
-    <row r="868" ht="15.75" customHeight="1"/>
-    <row r="869" ht="15.75" customHeight="1"/>
-    <row r="870" ht="15.75" customHeight="1"/>
-    <row r="871" ht="15.75" customHeight="1"/>
-    <row r="872" ht="15.75" customHeight="1"/>
-    <row r="873" ht="15.75" customHeight="1"/>
-    <row r="874" ht="15.75" customHeight="1"/>
-    <row r="875" ht="15.75" customHeight="1"/>
-    <row r="876" ht="15.75" customHeight="1"/>
-    <row r="877" ht="15.75" customHeight="1"/>
-    <row r="878" ht="15.75" customHeight="1"/>
-    <row r="879" ht="15.75" customHeight="1"/>
-    <row r="880" ht="15.75" customHeight="1"/>
-    <row r="881" ht="15.75" customHeight="1"/>
-    <row r="882" ht="15.75" customHeight="1"/>
-    <row r="883" ht="15.75" customHeight="1"/>
-    <row r="884" ht="15.75" customHeight="1"/>
-    <row r="885" ht="15.75" customHeight="1"/>
-    <row r="886" ht="15.75" customHeight="1"/>
-    <row r="887" ht="15.75" customHeight="1"/>
-    <row r="888" ht="15.75" customHeight="1"/>
-    <row r="889" ht="15.75" customHeight="1"/>
-    <row r="890" ht="15.75" customHeight="1"/>
-    <row r="891" ht="15.75" customHeight="1"/>
-    <row r="892" ht="15.75" customHeight="1"/>
-    <row r="893" ht="15.75" customHeight="1"/>
-    <row r="894" ht="15.75" customHeight="1"/>
-    <row r="895" ht="15.75" customHeight="1"/>
-    <row r="896" ht="15.75" customHeight="1"/>
-    <row r="897" ht="15.75" customHeight="1"/>
-    <row r="898" ht="15.75" customHeight="1"/>
-    <row r="899" ht="15.75" customHeight="1"/>
-    <row r="900" ht="15.75" customHeight="1"/>
-    <row r="901" ht="15.75" customHeight="1"/>
-    <row r="902" ht="15.75" customHeight="1"/>
-    <row r="903" ht="15.75" customHeight="1"/>
-    <row r="904" ht="15.75" customHeight="1"/>
-    <row r="905" ht="15.75" customHeight="1"/>
-    <row r="906" ht="15.75" customHeight="1"/>
-    <row r="907" ht="15.75" customHeight="1"/>
-    <row r="908" ht="15.75" customHeight="1"/>
-    <row r="909" ht="15.75" customHeight="1"/>
-    <row r="910" ht="15.75" customHeight="1"/>
-    <row r="911" ht="15.75" customHeight="1"/>
-    <row r="912" ht="15.75" customHeight="1"/>
-    <row r="913" ht="15.75" customHeight="1"/>
-    <row r="914" ht="15.75" customHeight="1"/>
-    <row r="915" ht="15.75" customHeight="1"/>
-    <row r="916" ht="15.75" customHeight="1"/>
-    <row r="917" ht="15.75" customHeight="1"/>
-    <row r="918" ht="15.75" customHeight="1"/>
-    <row r="919" ht="15.75" customHeight="1"/>
-    <row r="920" ht="15.75" customHeight="1"/>
-    <row r="921" ht="15.75" customHeight="1"/>
-    <row r="922" ht="15.75" customHeight="1"/>
-    <row r="923" ht="15.75" customHeight="1"/>
-    <row r="924" ht="15.75" customHeight="1"/>
-    <row r="925" ht="15.75" customHeight="1"/>
-    <row r="926" ht="15.75" customHeight="1"/>
-    <row r="927" ht="15.75" customHeight="1"/>
-    <row r="928" ht="15.75" customHeight="1"/>
-    <row r="929" ht="15.75" customHeight="1"/>
-    <row r="930" ht="15.75" customHeight="1"/>
-    <row r="931" ht="15.75" customHeight="1"/>
-    <row r="932" ht="15.75" customHeight="1"/>
-    <row r="933" ht="15.75" customHeight="1"/>
-    <row r="934" ht="15.75" customHeight="1"/>
-    <row r="935" ht="15.75" customHeight="1"/>
-    <row r="936" ht="15.75" customHeight="1"/>
-    <row r="937" ht="15.75" customHeight="1"/>
-    <row r="938" ht="15.75" customHeight="1"/>
-    <row r="939" ht="15.75" customHeight="1"/>
-    <row r="940" ht="15.75" customHeight="1"/>
-    <row r="941" ht="15.75" customHeight="1"/>
-    <row r="942" ht="15.75" customHeight="1"/>
-    <row r="943" ht="15.75" customHeight="1"/>
-    <row r="944" ht="15.75" customHeight="1"/>
-    <row r="945" ht="15.75" customHeight="1"/>
-    <row r="946" ht="15.75" customHeight="1"/>
-    <row r="947" ht="15.75" customHeight="1"/>
-    <row r="948" ht="15.75" customHeight="1"/>
-    <row r="949" ht="15.75" customHeight="1"/>
-    <row r="950" ht="15.75" customHeight="1"/>
-    <row r="951" ht="15.75" customHeight="1"/>
-    <row r="952" ht="15.75" customHeight="1"/>
-    <row r="953" ht="15.75" customHeight="1"/>
-    <row r="954" ht="15.75" customHeight="1"/>
-    <row r="955" ht="15.75" customHeight="1"/>
-    <row r="956" ht="15.75" customHeight="1"/>
-    <row r="957" ht="15.75" customHeight="1"/>
-    <row r="958" ht="15.75" customHeight="1"/>
-    <row r="959" ht="15.75" customHeight="1"/>
-    <row r="960" ht="15.75" customHeight="1"/>
-    <row r="961" ht="15.75" customHeight="1"/>
-    <row r="962" ht="15.75" customHeight="1"/>
-    <row r="963" ht="15.75" customHeight="1"/>
-    <row r="964" ht="15.75" customHeight="1"/>
-    <row r="965" ht="15.75" customHeight="1"/>
-    <row r="966" ht="15.75" customHeight="1"/>
-    <row r="967" ht="15.75" customHeight="1"/>
-    <row r="968" ht="15.75" customHeight="1"/>
-    <row r="969" ht="15.75" customHeight="1"/>
-    <row r="970" ht="15.75" customHeight="1"/>
-    <row r="971" ht="15.75" customHeight="1"/>
-    <row r="972" ht="15.75" customHeight="1"/>
-    <row r="973" ht="15.75" customHeight="1"/>
-    <row r="974" ht="15.75" customHeight="1"/>
-    <row r="975" ht="15.75" customHeight="1"/>
-    <row r="976" ht="15.75" customHeight="1"/>
-    <row r="977" ht="15.75" customHeight="1"/>
-    <row r="978" ht="15.75" customHeight="1"/>
-    <row r="979" ht="15.75" customHeight="1"/>
-    <row r="980" ht="15.75" customHeight="1"/>
-    <row r="981" ht="15.75" customHeight="1"/>
-    <row r="982" ht="15.75" customHeight="1"/>
-    <row r="983" ht="15.75" customHeight="1"/>
-    <row r="984" ht="15.75" customHeight="1"/>
-    <row r="985" ht="15.75" customHeight="1"/>
-    <row r="986" ht="15.75" customHeight="1"/>
-    <row r="987" ht="15.75" customHeight="1"/>
-    <row r="988" ht="15.75" customHeight="1"/>
-    <row r="989" ht="15.75" customHeight="1"/>
-    <row r="990" ht="15.75" customHeight="1"/>
-    <row r="991" ht="15.75" customHeight="1"/>
-    <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
-    <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="4" customHeight="1" spans="1:2">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customHeight="1" spans="1:2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="1" orientation="landscape"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -2340,72 +1286,63 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B1000"/>
+  <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="27.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="19.1428571428571" customWidth="1"/>
     <col min="3" max="26" width="9.14285714285714" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="4" t="s">
+    <row r="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" t="s">
         <v>7</v>
       </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="5" t="s">
+    <row r="2" customFormat="1" customHeight="1" spans="1:3">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="6" t="s">
+    <row r="3" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" customFormat="1" customHeight="1" spans="1:2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-    </row>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
     <row r="23" ht="15.75" customHeight="1"/>
@@ -3388,10 +2325,7 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="Nirvana"/>
-    <hyperlink ref="B2" r:id="rId2" display="archanachaya"/>
-    <hyperlink ref="A3" r:id="rId1" display="Nirvana"/>
-    <hyperlink ref="B3" r:id="rId2" display="asde@1235"/>
+    <hyperlink ref="C2" r:id="rId1" display="ninja@123" tooltip="mailto:ninja@123"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup paperSize="1" orientation="landscape"/>
@@ -3404,223 +2338,107 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1" outlineLevelCol="2"/>
-  <cols>
-    <col min="1" max="1" width="35.8571428571429" customWidth="1"/>
-    <col min="3" max="3" width="18.1428571428571" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" customHeight="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" customHeight="1" spans="1:1">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" customHeight="1" spans="1:1">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" customHeight="1" spans="1:3">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" customHeight="1" spans="1:3">
-      <c r="A5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" customHeight="1" spans="1:3">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" customHeight="1" spans="1:3">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7">
-        <v>1234567890</v>
-      </c>
-      <c r="C7">
-        <v>1234567890</v>
-      </c>
-    </row>
-    <row r="8" customHeight="1" spans="1:3">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" customHeight="1" spans="1:3">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" customHeight="1" spans="1:3">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" customHeight="1" spans="1:3">
-      <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" customHeight="1" spans="1:3">
-      <c r="A12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" customHeight="1" spans="1:3">
-      <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1" outlineLevelRow="6" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="36.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="35.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:2">
+    <row r="1" customHeight="1" spans="1:4">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="2" customHeight="1" spans="1:2">
+    <row r="2" customHeight="1" spans="1:3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:2">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customHeight="1" spans="1:2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" ht="142" customHeight="1" spans="1:2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" ht="102" customHeight="1" spans="1:2">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" ht="142" customHeight="1" spans="1:2">
-      <c r="A4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>35</v>
+    <row r="7" ht="151" customHeight="1" spans="1:2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="5" ht="102" customHeight="1" spans="1:2">
-      <c r="A5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>37</v>
+    <row r="8" ht="129" customHeight="1" spans="1:2">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="6" ht="151" customHeight="1" spans="1:2">
-      <c r="A6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" ht="129" customHeight="1" spans="1:2">
-      <c r="A7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>41</v>
+    <row r="9" customHeight="1" spans="1:3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C9" r:id="rId1" display="ninja@123" tooltip="mailto:ninja@123"/>
+    <hyperlink ref="C2" r:id="rId1" display="ninja@123" tooltip="mailto:ninja@123"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>